<commit_message>
Update Zero CO2 scenarios names and variants
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_ZeroCO2_CAP21-LAM.xlsx
+++ b/SuppXLS/Scen_SYS_ZeroCO2_CAP21-LAM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BCEC453-38C1-4520-8879-A5E149E0C051}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2A37CA7-4B78-408C-8EBC-966D5BC0A6C4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
@@ -50,6 +50,24 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={D7F7A51F-98CC-4BD8-BF17-ABDD25DA4C1B}</author>
+  </authors>
+  <commentList>
+    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{D7F7A51F-98CC-4BD8-BF17-ABDD25DA4C1B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    i.e. &gt;60% reduction from the 2018 value (ca. 40 Mt based on https://www.epa.ie/pubs/reports/air/airemissions/ghg2018/Ireland%20GHG%201990-2018%20Final%20Inventory_April%202020.pdf )</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
@@ -802,6 +820,12 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Balyk, Olexandr" id="{1B80334F-2539-4DC6-A837-54D1ADCF10B1}" userId="Balyk, Olexandr" providerId="None"/>
+</personList>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1121,6 +1145,14 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="D7" dT="2021-03-03T22:33:41.43" personId="{1B80334F-2539-4DC6-A837-54D1ADCF10B1}" id="{D7F7A51F-98CC-4BD8-BF17-ABDD25DA4C1B}">
+    <text>i.e. &gt;60% reduction from the 2018 value (ca. 40 Mt based on https://www.epa.ie/pubs/reports/air/airemissions/ghg2018/Ireland%20GHG%201990-2018%20Final%20Inventory_April%202020.pdf )</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42C030FF-C503-4743-9DBD-437AEB1E949D}">
   <sheetPr codeName="Sheet8"/>
@@ -1889,11 +1921,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{011941A8-04BF-45E8-9F60-D4E07475AB4A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{011941A8-04BF-45E8-9F60-D4E07475AB4A}">
   <dimension ref="A1:R17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="C14:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1901,18 +1933,18 @@
     <col min="1" max="1" width="9.140625" style="8"/>
     <col min="2" max="2" width="14" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" style="8" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="13" width="9.140625" style="8"/>
-    <col min="14" max="14" width="10.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12" style="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="8"/>
+    <col min="4" max="5" width="16.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="9.140625" style="8"/>
+    <col min="13" max="13" width="10.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1"/>
       <c r="B1"/>
       <c r="C1"/>
+      <c r="D1"/>
       <c r="E1"/>
       <c r="F1"/>
       <c r="G1"/>
@@ -1926,12 +1958,12 @@
       <c r="O1"/>
       <c r="P1"/>
       <c r="Q1"/>
-      <c r="R1"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2"/>
       <c r="B2"/>
       <c r="C2"/>
+      <c r="D2"/>
       <c r="E2"/>
       <c r="F2"/>
       <c r="G2"/>
@@ -1945,12 +1977,12 @@
       <c r="O2"/>
       <c r="P2"/>
       <c r="Q2"/>
-      <c r="R2"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="B3"/>
       <c r="C3"/>
+      <c r="D3"/>
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3"/>
@@ -1964,7 +1996,6 @@
       <c r="O3"/>
       <c r="P3"/>
       <c r="Q3"/>
-      <c r="R3"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4"/>
@@ -1972,9 +2003,10 @@
         <v>61</v>
       </c>
       <c r="C4" s="8" t="str">
-        <f xml:space="preserve"> _xlfn.TEXTJOIN("_",TRUE,"UC","NetZero","CO2","2050","LAM")</f>
-        <v>UC_NetZero_CO2_2050_LAM</v>
-      </c>
+        <f xml:space="preserve"> _xlfn.TEXTJOIN("_",TRUE,"UC","NetZero","CO2","2050")</f>
+        <v>UC_NetZero_CO2_2050</v>
+      </c>
+      <c r="E4"/>
       <c r="F4"/>
       <c r="G4"/>
       <c r="H4"/>
@@ -1987,7 +2019,6 @@
       <c r="O4"/>
       <c r="P4"/>
       <c r="Q4"/>
-      <c r="R4"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5"/>
@@ -1995,9 +2026,10 @@
         <v>66</v>
       </c>
       <c r="C5" t="str">
-        <f xml:space="preserve"> _xlfn.TEXTJOIN(" ",TRUE,"Net Zero CO2 by 2050 - LAM")</f>
-        <v>Net Zero CO2 by 2050 - LAM</v>
-      </c>
+        <f xml:space="preserve"> _xlfn.TEXTJOIN(" ",TRUE,"Net Zero CO2 by 2050")</f>
+        <v>Net Zero CO2 by 2050</v>
+      </c>
+      <c r="E5"/>
       <c r="F5"/>
       <c r="G5"/>
       <c r="H5"/>
@@ -2010,7 +2042,6 @@
       <c r="O5"/>
       <c r="P5"/>
       <c r="Q5"/>
-      <c r="R5"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
@@ -2033,11 +2064,11 @@
       <c r="B7" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C7">
-        <v>25989</v>
-      </c>
-      <c r="D7">
-        <v>11970</v>
+      <c r="C7" s="8">
+        <v>28095</v>
+      </c>
+      <c r="D7" s="8">
+        <v>15724</v>
       </c>
       <c r="E7" s="8">
         <v>0</v>
@@ -2070,7 +2101,7 @@
         <v>76</v>
       </c>
       <c r="D9" s="8" t="str">
-        <f t="shared" ref="D9:E12" si="0">C9</f>
+        <f t="shared" ref="D9:E9" si="0">C9</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="E9" s="8" t="str">
@@ -2086,11 +2117,11 @@
         <v>75</v>
       </c>
       <c r="D10" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D10:E12" si="1">C10</f>
         <v>ENV</v>
       </c>
       <c r="E10" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>ENV</v>
       </c>
     </row>
@@ -2107,11 +2138,11 @@
         <v>68</v>
       </c>
       <c r="D12" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>UP</v>
       </c>
       <c r="E12" s="8" t="str">
-        <f t="shared" ref="E12" si="1">D12</f>
+        <f t="shared" si="1"/>
         <v>UP</v>
       </c>
     </row>
@@ -2136,7 +2167,7 @@
       <c r="B14" t="s">
         <v>86</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="8">
         <v>1</v>
       </c>
       <c r="D14" s="8">
@@ -2165,6 +2196,7 @@
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15"/>
+      <c r="D15"/>
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15"/>
@@ -2178,12 +2210,12 @@
       <c r="O15"/>
       <c r="P15"/>
       <c r="Q15"/>
-      <c r="R15"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16"/>
+      <c r="D16"/>
       <c r="E16"/>
       <c r="F16"/>
       <c r="G16"/>
@@ -2197,12 +2229,12 @@
       <c r="O16"/>
       <c r="P16"/>
       <c r="Q16"/>
-      <c r="R16"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17"/>
       <c r="B17"/>
       <c r="C17"/>
+      <c r="D17"/>
       <c r="E17"/>
       <c r="F17"/>
       <c r="G17"/>
@@ -2216,11 +2248,11 @@
       <c r="O17"/>
       <c r="P17"/>
       <c r="Q17"/>
-      <c r="R17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2228,8 +2260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9318C9B-7F0A-410C-BCB5-F22D93E1F454}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2240,11 +2272,11 @@
     <col min="4" max="4" width="8.85546875" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="8"/>
     <col min="8" max="8" width="12.42578125" style="8" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.28515625" style="8" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.85546875" style="8" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
@@ -2321,7 +2353,7 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="str">
         <f>VLOOKUP(B$5, config!$B$4:$F$14,2,FALSE) &amp; "_Single"</f>
-        <v>UC_NetZero_CO2_2050_LAM_Single</v>
+        <v>UC_NetZero_CO2_2050_Single</v>
       </c>
       <c r="C7" s="8" t="str">
         <f>VLOOKUP(C$5, config!$B$4:$F$14,2,FALSE)</f>
@@ -2345,11 +2377,11 @@
       </c>
       <c r="J7" s="8">
         <f>VLOOKUP("Value", config!$B$4:$F$14,2,FALSE)</f>
-        <v>25989</v>
+        <v>28095</v>
       </c>
       <c r="K7" s="8" t="str">
         <f>VLOOKUP(K$5, config!$B$4:$F$14,2,FALSE) &amp; " - Single"</f>
-        <v>Net Zero CO2 by 2050 - LAM - Single</v>
+        <v>Net Zero CO2 by 2050 - Single</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -2397,7 +2429,7 @@
       </c>
       <c r="J9" s="8">
         <f>VLOOKUP("Value", config!$B$4:$F$14,3,FALSE)</f>
-        <v>11970</v>
+        <v>15724</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -2491,13 +2523,13 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="8"/>
-    <col min="2" max="2" width="27.42578125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" style="8" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.85546875" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" style="8" bestFit="1" customWidth="1"/>
@@ -2583,7 +2615,7 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="str">
         <f>VLOOKUP(B$5, config!$B$4:$F$14,2,FALSE) &amp; "_Multi"</f>
-        <v>UC_NetZero_CO2_2050_LAM_Multi</v>
+        <v>UC_NetZero_CO2_2050_Multi</v>
       </c>
       <c r="C7" s="8" t="str">
         <f>VLOOKUP(C$5, config!$B$4:$F$14,2,FALSE)</f>
@@ -2607,11 +2639,11 @@
       </c>
       <c r="J7" s="8">
         <f>VLOOKUP("Value", config!$B$4:$F$14,2,FALSE)</f>
-        <v>25989</v>
+        <v>28095</v>
       </c>
       <c r="K7" s="8" t="str">
         <f>VLOOKUP(K$5, config!$B$4:$F$14,2,FALSE) &amp; " - Multi"</f>
-        <v>Net Zero CO2 by 2050 - LAM - Multi</v>
+        <v>Net Zero CO2 by 2050 - Multi</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -2659,7 +2691,7 @@
       </c>
       <c r="J9" s="8">
         <f>VLOOKUP("Value", config!$B$4:$F$14,3,FALSE)</f>
-        <v>11970</v>
+        <v>15724</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -2753,7 +2785,7 @@
   <dimension ref="B2:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>